<commit_message>
fix foundation bag with average ground params calculations
</commit_message>
<xml_diff>
--- a/core/static/Расчет_сваи.xlsx
+++ b/core/static/Расчет_сваи.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\YandexDisk\Удаленка\Общий диск\AMAST-автоматизация\amast_ta\core\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64687224-DA07-4D1A-9116-E0059A6C60DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0090581D-BDBA-4117-9675-BE427A6F0836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Интерфейс" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="386">
   <si>
     <t>* блок "Геометрические характеристики сваи" *</t>
   </si>
@@ -3719,8 +3719,12 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="M6" s="1" t="s">
@@ -3744,8 +3748,12 @@
       <c r="D7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="M7" s="1" t="s">
@@ -3771,8 +3779,12 @@
       <c r="D8" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>154</v>
+      </c>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
       <c r="M8" s="29" t="s">
@@ -3796,8 +3808,12 @@
       <c r="D9" s="8">
         <v>0</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="E9" s="8">
+        <v>5</v>
+      </c>
+      <c r="F9" s="8">
+        <v>13</v>
+      </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="M9" s="1" t="s">
@@ -3813,10 +3829,14 @@
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="8">
-        <v>15</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>13</v>
+      </c>
+      <c r="F10" s="8">
+        <v>17</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="M10" s="1" t="s">
@@ -3833,15 +3853,15 @@
       <c r="C11" s="29"/>
       <c r="D11" s="56">
         <f>D10-D9</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E11" s="56">
         <f>IF(E7="нет грунта","данный слой отсутствует",E10-E9)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F11" s="56">
         <f>IF(F7="нет грунта","данный слой отсутствует",F10-F9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G11" s="56">
         <f>IF(G7="нет грунта","данный слой отсутствует",G10-G9)</f>
@@ -3875,8 +3895,12 @@
       <c r="D13" s="1">
         <v>0.8</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="E13" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.4</v>
+      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
@@ -3888,8 +3912,12 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="J14" s="1" t="s">
@@ -3918,8 +3946,12 @@
       <c r="D15" s="1">
         <v>25</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1">
+        <v>15</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="J15" s="1" t="s">
@@ -3937,7 +3969,7 @@
 IF($B$3&lt;=$H$10,
 (D15*$D$11+E15*$E$11+F15*$F$11+G15*$G$11+H15*($B$3-$H$9))/$B$3,
 1))))),1)</f>
-        <v>25</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -3948,8 +3980,12 @@
       <c r="D16" s="8">
         <v>1.88</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
+      <c r="E16" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
@@ -3960,23 +3996,23 @@
       <c r="C17" s="1"/>
       <c r="D17" s="30">
         <f>ROUND(IF($B$23&lt;$B$3,(2.72-1)/(1+D13)*($B$3-$B$23)/$B$3+D16*$B$23/$B$3,D16),2)</f>
-        <v>1.63</v>
+        <v>1.88</v>
       </c>
       <c r="E17" s="30">
         <f>ROUND(IF($B$23&lt;$B$3,(2.72-1)/(1+E13)*($B$3-$B$23)/$B$3+E16*$B$23/$B$3,E16),2)</f>
-        <v>0.47</v>
+        <v>1.33</v>
       </c>
       <c r="F17" s="30">
         <f>ROUND(IF($B$23&lt;$B$3,(2.72-1)/(1+F13)*($B$3-$B$23)/$B$3+F16*$B$23/$B$3,F16),2)</f>
-        <v>0.47</v>
+        <v>1</v>
       </c>
       <c r="G17" s="30">
         <f>ROUND(IF($B$23&lt;$B$3,(2.72-1)/(1+G13)*($B$3-$B$23)/$B$3+G16*$B$23/$B$3,G16),2)</f>
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="H17" s="30">
         <f>ROUND(IF($B$23&lt;$B$3,(2.72-1)/(1+H13)*($B$3-$B$23)/$B$3+H16*$B$23/$B$3,H16),2)</f>
-        <v>0.47</v>
+        <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>163</v>
@@ -3993,7 +4029,7 @@
 IF($B$3&lt;=$H$10,
 (D17*$D$11+E17*$E$11+F17*$F$11+G17*$G$11+H17*($B$3-$H$9))/$B$3,
 1))))),2)</f>
-        <v>1.63</v>
+        <v>1.58</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
@@ -4002,10 +4038,14 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1">
-        <v>8000000</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+        <v>8000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>9000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>10000</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="J18" s="1" t="s">
@@ -4023,7 +4063,7 @@
 IF($B$3&lt;=$H$10,
 (D18*$D$11+E18*$E$11+F18*$F$11+G18*$G$11+H18*($B$3-$H$9))/$B$3,
 1))))),0)</f>
-        <v>8000000</v>
+        <v>8545</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
@@ -4037,13 +4077,13 @@
         <f>MATCH(D7,$M$6:$M$10,0)</f>
         <v>3</v>
       </c>
-      <c r="E19" s="56" t="e">
+      <c r="E19" s="56">
         <f>MATCH(E7,$M$6:$M$10,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F19" s="56" t="e">
+        <v>4</v>
+      </c>
+      <c r="F19" s="56">
         <f>MATCH(F7,$M$6:$M$10,0)</f>
-        <v>#N/A</v>
+        <v>2</v>
       </c>
       <c r="G19" s="56" t="e">
         <f>MATCH(G7,$M$6:$M$10,0)</f>
@@ -4063,13 +4103,13 @@
         <f ca="1">OFFSET($N$5,D19,0)</f>
         <v>1.25</v>
       </c>
-      <c r="E20" s="57" t="e">
+      <c r="E20" s="57">
         <f ca="1">OFFSET($N$5,E19,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F20" s="57" t="e">
+        <v>1.3</v>
+      </c>
+      <c r="F20" s="57">
         <f ca="1">OFFSET($N$5,F19,0)</f>
-        <v>#N/A</v>
+        <v>1.2</v>
       </c>
       <c r="G20" s="57" t="e">
         <f ca="1">OFFSET($N$5,G19,0)</f>
@@ -4087,7 +4127,7 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
@@ -4118,7 +4158,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C28" s="63">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="D28" s="110"/>
     </row>
@@ -4232,7 +4272,7 @@
       </c>
       <c r="M3" s="24">
         <f>I8*1000</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N3" s="122"/>
       <c r="R3" s="38" t="s">
@@ -4409,11 +4449,11 @@
       </c>
       <c r="I8" s="24">
         <f>J8/1000</f>
-        <v>1.6E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="J8" s="17">
         <f>'Расчет массы фланца'!C4</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K8" s="37"/>
       <c r="L8" s="125" t="s">
@@ -4432,7 +4472,7 @@
       </c>
       <c r="D9" s="27">
         <f>IF(Интерфейс!B8 = "Исходных данных нет",'Типовые грунты'!D24,'Задание грунтов'!K15)</f>
-        <v>25</v>
+        <v>23.9</v>
       </c>
       <c r="E9" s="120" t="s">
         <v>197</v>
@@ -4454,7 +4494,7 @@
       </c>
       <c r="M9" s="22">
         <f>M8*M3</f>
-        <v>87458.539049759071</v>
+        <v>98390.856430978951</v>
       </c>
       <c r="N9" s="122"/>
       <c r="R9" s="1" t="s">
@@ -4468,7 +4508,7 @@
       </c>
       <c r="D10" s="25">
         <f>RADIANS(D9)</f>
-        <v>0.43633231299858238</v>
+        <v>0.41713369122664473</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>210</v>
@@ -4478,7 +4518,7 @@
       </c>
       <c r="I10" s="26">
         <f>PI()/64*(I6^4-(I6-2*I8)^4)</f>
-        <v>3.0008572245490018E-2</v>
+        <v>3.3640318509671453E-2</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="37"/>
@@ -4487,7 +4527,7 @@
       </c>
       <c r="M10" s="23">
         <f>M4*M9*10^(-9)</f>
-        <v>1.0057731990722294</v>
+        <v>1.131494848956258</v>
       </c>
       <c r="N10" s="122"/>
       <c r="R10" s="42" t="s">
@@ -4514,7 +4554,7 @@
       </c>
       <c r="M11" s="21">
         <f>M5*M10</f>
-        <v>7895.3196127170004</v>
+        <v>8882.2345643066255</v>
       </c>
       <c r="N11" s="122"/>
       <c r="R11" s="43" t="s">
@@ -4553,7 +4593,7 @@
       </c>
       <c r="D13" s="18">
         <f>IF(Интерфейс!B8 = "Исходных данных нет",'Типовые грунты'!F24,'Задание грунтов'!K17)</f>
-        <v>1.63</v>
+        <v>1.58</v>
       </c>
       <c r="E13" s="120" t="s">
         <v>197</v>
@@ -4612,7 +4652,7 @@
       </c>
       <c r="D15" s="62">
         <f>IF(Интерфейс!B8 = "Исходных данных нет",'Типовые грунты'!G24,'Задание грунтов'!K18)</f>
-        <v>8000000</v>
+        <v>8545</v>
       </c>
       <c r="E15" s="120" t="s">
         <v>197</v>
@@ -4642,7 +4682,7 @@
       </c>
       <c r="D16" s="24">
         <f>'Задание грунтов'!B23</f>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E16" s="120" t="s">
         <v>188</v>
@@ -4773,7 +4813,7 @@
       </c>
       <c r="D23" s="2">
         <f>D9</f>
-        <v>25</v>
+        <v>23.9</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>80</v>
@@ -4798,14 +4838,14 @@
       </c>
       <c r="D24" s="2">
         <f>RADIANS(D23)</f>
-        <v>0.43633231299858238</v>
+        <v>0.41713369122664473</v>
       </c>
       <c r="G24" s="39" t="s">
         <v>242</v>
       </c>
       <c r="H24" s="2">
         <f>I7+2/I31</f>
-        <v>7.4052339532180707</v>
+        <v>7.564824055702454</v>
       </c>
       <c r="I24" s="37"/>
       <c r="J24" s="37"/>
@@ -4828,14 +4868,14 @@
       </c>
       <c r="D25" s="25">
         <f>0.9*((TAN(D24)-0.1))</f>
-        <v>0.32967689233949871</v>
+        <v>0.30882510325968021</v>
       </c>
       <c r="G25" s="39" t="s">
         <v>247</v>
       </c>
       <c r="H25" s="2">
         <f>(I15+I16*H24)/I10*I6/2/1000</f>
-        <v>219.09423852206814</v>
+        <v>196.61490524542123</v>
       </c>
       <c r="I25" s="37"/>
       <c r="J25" s="37"/>
@@ -4858,14 +4898,14 @@
       </c>
       <c r="D26" s="2">
         <f>D13</f>
-        <v>1.63</v>
+        <v>1.58</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>252</v>
       </c>
       <c r="H26" s="48">
         <f>H25/235</f>
-        <v>0.93231590860454527</v>
+        <v>0.83665917125711164</v>
       </c>
       <c r="I26" s="37" t="s">
         <v>253</v>
@@ -4885,14 +4925,14 @@
       </c>
       <c r="D27" s="2">
         <f>DEGREES(D28)</f>
-        <v>25</v>
+        <v>23.9</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>256</v>
       </c>
       <c r="H27" s="48">
         <f>H25/335</f>
-        <v>0.65401265230468097</v>
+        <v>0.58691016491170511</v>
       </c>
       <c r="I27" s="37" t="s">
         <v>253</v>
@@ -4910,7 +4950,7 @@
       </c>
       <c r="D28" s="2">
         <f>ATAN(TAN(D24)+D22/10)</f>
-        <v>0.43633231299858238</v>
+        <v>0.41713369122664473</v>
       </c>
       <c r="G28" s="37"/>
       <c r="H28" s="37"/>
@@ -4930,7 +4970,7 @@
       </c>
       <c r="D29" s="2">
         <f>D15/9.8</f>
-        <v>816326.53061224485</v>
+        <v>871.93877551020398</v>
       </c>
       <c r="G29" s="37"/>
       <c r="H29" s="37"/>
@@ -4975,7 +5015,7 @@
       </c>
       <c r="I31" s="23">
         <f>(D11*I30/D14/I9/I10)^0.2</f>
-        <v>0.28963537130670758</v>
+        <v>0.28309268344562338</v>
       </c>
       <c r="J31" s="37"/>
       <c r="K31" s="37"/>
@@ -5002,7 +5042,7 @@
       </c>
       <c r="I32" s="23">
         <f>I5*I31</f>
-        <v>3.1859890843737833</v>
+        <v>3.1140195179018573</v>
       </c>
       <c r="J32" s="37"/>
       <c r="K32" s="37"/>
@@ -5371,7 +5411,7 @@
       </c>
       <c r="D65" s="23">
         <f>(D51/2+D53)*D25/D50</f>
-        <v>2.5475032589870352E-2</v>
+        <v>2.3863757979157105E-2</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5381,7 +5421,7 @@
       </c>
       <c r="D66" s="23">
         <f>(D51/2+D54)*D25/D50</f>
-        <v>2.5475032589870352E-2</v>
+        <v>2.3863757979157105E-2</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
@@ -5391,7 +5431,7 @@
       </c>
       <c r="D67" s="23">
         <f>D26*TAN(RADIANS(45+D23/2))^2</f>
-        <v>4.0161778819473897</v>
+        <v>3.7321884632916644</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5421,7 +5461,7 @@
       </c>
       <c r="D70" s="50">
         <f>D25*D51/2/D50</f>
-        <v>2.5475032589870352E-2</v>
+        <v>2.3863757979157105E-2</v>
       </c>
     </row>
     <row r="71" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5431,7 +5471,7 @@
       </c>
       <c r="D71" s="23">
         <f>2/3*TAN(D28/5)/TAN(RADIANS(45-D27/2))</f>
-        <v>9.1553128865285299E-2</v>
+        <v>8.5679406680574513E-2</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5441,7 +5481,7 @@
       </c>
       <c r="D72" s="23">
         <f>1+D71*D50/D51</f>
-        <v>1.5924025985400814</v>
+        <v>1.5543961608743055</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
@@ -5453,7 +5493,7 @@
       </c>
       <c r="D73" s="23">
         <f>D51*D72</f>
-        <v>2.7070844175181383</v>
+        <v>2.6424734734863193</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
@@ -5465,7 +5505,7 @@
       </c>
       <c r="D74" s="22">
         <f>D67*D73*D50*D50/2</f>
-        <v>657.76402001314727</v>
+        <v>596.66364524414348</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
@@ -5519,7 +5559,7 @@
       </c>
       <c r="D79" s="20">
         <f>D25*D43/D74</f>
-        <v>1.0938107511075899E-2</v>
+        <v>1.1295535166048549E-2</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
@@ -5565,7 +5605,7 @@
       </c>
       <c r="D84" s="2">
         <f>-(1/4*((2*D69+1)*(3*D64+3*D70+2)-D69)+3/4*D79*(1+D64)-3/4*(D77*(D64+D55/D50-D65)-D78*(D64-D56/D50+D66+1)))</f>
-        <v>-1.8486423933308607</v>
+        <v>-1.8481691789399233</v>
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.3">
@@ -5585,7 +5625,7 @@
       </c>
       <c r="D86" s="23">
         <f>(-1/4*(((2*D69+1)*(3*D64+3*D70+2)-D69)-3*(D77*(D64+D55/D50-D65)-D78*(D64-D56/D50+D66+1))+3*D79*(1+D64))+0.03125)/(3/2*(D64+D69)+1.5)</f>
-        <v>-0.44175025623045522</v>
+        <v>-0.44163523287104445</v>
       </c>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.3">
@@ -5597,7 +5637,7 @@
       </c>
       <c r="D87" s="50">
         <f>-D85/2+SQRT((D85/2)^2-D86)</f>
-        <v>0.73651241836870818</v>
+        <v>0.73642633675780655</v>
       </c>
     </row>
     <row r="88" spans="2:13" x14ac:dyDescent="0.3">
@@ -5642,7 +5682,7 @@
       </c>
       <c r="D92" s="25">
         <f>IF(Интерфейс!B8 = "Исходных данных нет",'Типовые грунты'!H24,'Задание грунтов'!C28)</f>
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="E92" s="121" t="s">
         <v>341</v>
@@ -5671,7 +5711,7 @@
       </c>
       <c r="D94" s="2">
         <f>D63/(D64+D87)*(D74*(2/3*(D87^3+3*D69*(D87^2-D87+1/2)-3/2*D87+1)+(2*D69+1)*D70)+D25*D43*(1-D87)+D75*(D87-D55/D50+D65)+D76*(1-D87-D56/D50+D66))*D47</f>
-        <v>59.657377238825099</v>
+        <v>53.750973908683619</v>
       </c>
     </row>
     <row r="95" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5681,7 +5721,7 @@
       </c>
       <c r="D95" s="2">
         <f>D94*D44</f>
-        <v>1143.6236820387676</v>
+        <v>1030.398745967886</v>
       </c>
     </row>
     <row r="96" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5693,7 +5733,7 @@
       </c>
       <c r="D96" s="2">
         <f>D94*D92/D93</f>
-        <v>57.362862729639517</v>
+        <v>53.750973908683619</v>
       </c>
     </row>
     <row r="97" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5705,7 +5745,7 @@
       </c>
       <c r="D97" s="2">
         <f>D96*D44</f>
-        <v>1099.6381558065073</v>
+        <v>1030.398745967886</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.3">
@@ -5715,7 +5755,7 @@
       <c r="C98" s="55"/>
       <c r="D98" s="53">
         <f>D41/D96</f>
-        <v>0.51775658652150813</v>
+        <v>0.55254812778753915</v>
       </c>
       <c r="E98" s="34" t="s">
         <v>253</v>
@@ -5802,7 +5842,7 @@
       </c>
       <c r="D107" s="111">
         <f>ROUND((3*D45/4/D29/D50/D50*(6*D64+3)*D104),3)</f>
-        <v>0</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="E107" s="34" t="s">
         <v>253</v>
@@ -5815,7 +5855,7 @@
       <c r="C108" s="41"/>
       <c r="D108" s="51">
         <f>3*D45/8/D29/D50/D50*((6*D64+5)*D105+(6*D64+1)*D106)</f>
-        <v>1.8800759803518353E-5</v>
+        <v>1.760164756327055E-2</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.3">
@@ -5934,7 +5974,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="88">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="91" t="s">
         <v>365</v>
@@ -6062,7 +6102,7 @@
       </c>
       <c r="C10" s="93">
         <f>C9*C4</f>
-        <v>87458.539049759071</v>
+        <v>98390.856430978951</v>
       </c>
       <c r="D10" s="86"/>
       <c r="E10" s="122"/>
@@ -6084,7 +6124,7 @@
       </c>
       <c r="C11" s="94">
         <f>C5*C10*10^(-9)</f>
-        <v>0.96204392954734985</v>
+        <v>1.0822994207407686</v>
       </c>
       <c r="D11" s="86"/>
       <c r="E11" s="122"/>
@@ -6106,7 +6146,7 @@
       </c>
       <c r="C12" s="96">
         <f>C6*C11</f>
-        <v>7552.0448469466965</v>
+        <v>8496.0504528150341</v>
       </c>
       <c r="D12" s="91" t="s">
         <v>374</v>
@@ -6132,7 +6172,7 @@
       </c>
       <c r="C13" s="96">
         <f>C12*1.1</f>
-        <v>8307.2493316413675</v>
+        <v>9345.6554980965375</v>
       </c>
       <c r="D13" s="91" t="s">
         <v>374</v>
@@ -6151,7 +6191,7 @@
       </c>
       <c r="C14" s="100">
         <f>C12*1.15</f>
-        <v>8684.8515739887007</v>
+        <v>9770.4580207372892</v>
       </c>
       <c r="D14" s="101" t="s">
         <v>374</v>
@@ -6176,7 +6216,7 @@
       </c>
       <c r="G15" s="35">
         <f>C12+G12</f>
-        <v>8024.6475692374806</v>
+        <v>8968.6531751058174</v>
       </c>
       <c r="H15" s="91" t="s">
         <v>374</v>
@@ -6195,7 +6235,7 @@
       </c>
       <c r="G16" s="35">
         <f>G15*1.1</f>
-        <v>8827.1123261612302</v>
+        <v>9865.5184926164002</v>
       </c>
       <c r="H16" s="91" t="s">
         <v>374</v>
@@ -6214,7 +6254,7 @@
       </c>
       <c r="G17" s="104">
         <f>G15*1.15</f>
-        <v>9228.3447046231013</v>
+        <v>10313.95115137169</v>
       </c>
       <c r="H17" s="101" t="s">
         <v>374</v>

</xml_diff>